<commit_message>
Created database classes and database helper class. Wrote functions for each database class as well as used these functions in the search page as well as results page for testing purposes. I have also created a rough draft of the form the we will use for the assignment in the search page to test the functionality so far
</commit_message>
<xml_diff>
--- a/hits-2016_to_2019.xlsx
+++ b/hits-2016_to_2019.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\web development textbook\third-edition\case-studies\case-music\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Applications/XAMPP/xamppfiles/htdocs/patwa172-assign1/patwa172-assign1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0CA7579-CA0F-48A2-B430-5D0213D3D77C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC05A027-0B7A-6447-A025-47F869456E34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-25710" yWindow="1620" windowWidth="21435" windowHeight="13695" xr2:uid="{F421C9D2-FE21-4230-9F31-BC5BBCAECA5E}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19720" xr2:uid="{F421C9D2-FE21-4230-9F31-BC5BBCAECA5E}"/>
   </bookViews>
   <sheets>
     <sheet name="songs" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="535" uniqueCount="527">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="536" uniqueCount="528">
   <si>
     <t>a lot</t>
   </si>
@@ -1620,6 +1620,9 @@
   </si>
   <si>
     <t>type_name</t>
+  </si>
+  <si>
+    <t>tit</t>
   </si>
 </sst>
 </file>
@@ -2015,20 +2018,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9AE7F33E-ABF3-4712-A988-A84BD037C015}">
   <dimension ref="A1:O318"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D17" sqref="D17"/>
+    <sheetView tabSelected="1" zoomScale="138" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A99" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A117" sqref="A117"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" width="11.7109375" customWidth="1"/>
-    <col min="8" max="8" width="10.28515625" customWidth="1"/>
-    <col min="13" max="13" width="12.140625" customWidth="1"/>
-    <col min="14" max="14" width="11.5703125" customWidth="1"/>
+    <col min="3" max="3" width="11.6640625" customWidth="1"/>
+    <col min="8" max="8" width="10.33203125" customWidth="1"/>
+    <col min="13" max="13" width="12.1640625" customWidth="1"/>
+    <col min="14" max="14" width="11.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>519</v>
       </c>
@@ -2075,7 +2078,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="2" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1001</v>
       </c>
@@ -2122,7 +2125,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="3" spans="1:15" ht="23.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>1002</v>
       </c>
@@ -2169,7 +2172,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="4" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>1003</v>
       </c>
@@ -2216,7 +2219,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="5" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>1004</v>
       </c>
@@ -2263,7 +2266,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="6" spans="1:15" ht="34.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:15" ht="25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>1005</v>
       </c>
@@ -2310,7 +2313,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="7" spans="1:15" ht="23.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:15" ht="25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>1006</v>
       </c>
@@ -2357,7 +2360,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="8" spans="1:15" ht="23.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:15" ht="25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>1007</v>
       </c>
@@ -2404,7 +2407,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="9" spans="1:15" ht="23.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:15" ht="25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>1008</v>
       </c>
@@ -2451,7 +2454,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="10" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>1009</v>
       </c>
@@ -2498,7 +2501,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="11" spans="1:15" ht="23.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:15" ht="25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>1010</v>
       </c>
@@ -2545,7 +2548,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="12" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>1011</v>
       </c>
@@ -2592,7 +2595,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="13" spans="1:15" ht="23.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:15" ht="25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>1012</v>
       </c>
@@ -2639,7 +2642,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="14" spans="1:15" ht="34.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:15" ht="25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>1014</v>
       </c>
@@ -2686,7 +2689,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="15" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>1015</v>
       </c>
@@ -2733,7 +2736,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="16" spans="1:15" ht="34.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:15" ht="37" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>1016</v>
       </c>
@@ -2780,7 +2783,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="17" spans="1:15" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:15" ht="25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>1017</v>
       </c>
@@ -2827,7 +2830,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="18" spans="1:15" ht="23.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:15" ht="25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>1018</v>
       </c>
@@ -2874,7 +2877,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="19" spans="1:15" ht="23.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>1019</v>
       </c>
@@ -2921,7 +2924,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="20" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>1020</v>
       </c>
@@ -2968,7 +2971,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="21" spans="1:15" ht="23.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>1021</v>
       </c>
@@ -3015,7 +3018,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="22" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>1022</v>
       </c>
@@ -3062,7 +3065,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="23" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>1023</v>
       </c>
@@ -3109,7 +3112,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="24" spans="1:15" ht="57" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:15" ht="49" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>1024</v>
       </c>
@@ -3156,7 +3159,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="25" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>1025</v>
       </c>
@@ -3203,7 +3206,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="26" spans="1:15" ht="34.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:15" ht="25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>1026</v>
       </c>
@@ -3250,7 +3253,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="27" spans="1:15" ht="23.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:15" ht="25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>1027</v>
       </c>
@@ -3297,7 +3300,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="28" spans="1:15" ht="23.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:15" ht="25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>1028</v>
       </c>
@@ -3344,7 +3347,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="29" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>1029</v>
       </c>
@@ -3391,7 +3394,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="30" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>1030</v>
       </c>
@@ -3438,7 +3441,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="31" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>1031</v>
       </c>
@@ -3485,7 +3488,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="32" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>1032</v>
       </c>
@@ -3532,7 +3535,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="33" spans="1:15" ht="23.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:15" ht="25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>1033</v>
       </c>
@@ -3579,7 +3582,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="34" spans="1:15" ht="23.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:15" ht="25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>1034</v>
       </c>
@@ -3626,7 +3629,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="35" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>1035</v>
       </c>
@@ -3673,7 +3676,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="36" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>1036</v>
       </c>
@@ -3720,7 +3723,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="37" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>1037</v>
       </c>
@@ -3767,7 +3770,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="38" spans="1:15" ht="34.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:15" ht="37" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>1038</v>
       </c>
@@ -3814,7 +3817,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="39" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>1039</v>
       </c>
@@ -3861,7 +3864,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="40" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>1040</v>
       </c>
@@ -3908,7 +3911,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="41" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>1041</v>
       </c>
@@ -3955,7 +3958,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="42" spans="1:15" ht="23.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:15" ht="25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <v>1042</v>
       </c>
@@ -4002,7 +4005,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="43" spans="1:15" ht="23.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:15" ht="25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <v>1043</v>
       </c>
@@ -4049,7 +4052,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="44" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <v>1044</v>
       </c>
@@ -4096,7 +4099,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="45" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
         <v>1045</v>
       </c>
@@ -4143,7 +4146,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="46" spans="1:15" ht="23.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
         <v>1046</v>
       </c>
@@ -4190,7 +4193,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="47" spans="1:15" ht="34.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:15" ht="37" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
         <v>1047</v>
       </c>
@@ -4237,7 +4240,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="48" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
         <v>1048</v>
       </c>
@@ -4284,7 +4287,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="49" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
         <v>1049</v>
       </c>
@@ -4331,7 +4334,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="50" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
         <v>1050</v>
       </c>
@@ -4378,7 +4381,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="51" spans="1:15" ht="23.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:15" ht="25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
         <v>1051</v>
       </c>
@@ -4425,7 +4428,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="52" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
         <v>1052</v>
       </c>
@@ -4472,7 +4475,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="53" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
         <v>1053</v>
       </c>
@@ -4519,7 +4522,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="54" spans="1:15" ht="34.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:15" ht="37" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
         <v>1054</v>
       </c>
@@ -4566,7 +4569,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="55" spans="1:15" ht="57" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:15" ht="49" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
         <v>1055</v>
       </c>
@@ -4613,7 +4616,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="56" spans="1:15" ht="23.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:15" ht="25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
         <v>1056</v>
       </c>
@@ -4660,7 +4663,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="57" spans="1:15" ht="68.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:15" ht="49" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
         <v>1057</v>
       </c>
@@ -4707,7 +4710,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="58" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
         <v>1058</v>
       </c>
@@ -4754,7 +4757,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="59" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A59" s="1">
         <v>1059</v>
       </c>
@@ -4801,7 +4804,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="60" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
         <v>1060</v>
       </c>
@@ -4848,7 +4851,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="61" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A61" s="1">
         <v>1061</v>
       </c>
@@ -4895,7 +4898,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="62" spans="1:15" ht="34.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:15" ht="25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A62" s="1">
         <v>1062</v>
       </c>
@@ -4942,7 +4945,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="63" spans="1:15" ht="23.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A63" s="1">
         <v>1063</v>
       </c>
@@ -4989,7 +4992,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="64" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A64" s="1">
         <v>1064</v>
       </c>
@@ -5036,7 +5039,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="65" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A65" s="1">
         <v>1065</v>
       </c>
@@ -5083,7 +5086,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="66" spans="1:15" ht="23.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:15" ht="25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A66" s="1">
         <v>1066</v>
       </c>
@@ -5130,7 +5133,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="67" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A67" s="1">
         <v>1067</v>
       </c>
@@ -5177,7 +5180,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="68" spans="1:15" ht="34.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:15" ht="25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A68" s="1">
         <v>1068</v>
       </c>
@@ -5224,7 +5227,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="69" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A69" s="1">
         <v>1069</v>
       </c>
@@ -5271,7 +5274,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="70" spans="1:15" ht="34.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:15" ht="25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A70" s="1">
         <v>1070</v>
       </c>
@@ -5318,7 +5321,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="71" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A71" s="1">
         <v>1071</v>
       </c>
@@ -5365,7 +5368,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="72" spans="1:15" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:15" ht="49" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A72" s="1">
         <v>1072</v>
       </c>
@@ -5412,7 +5415,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="73" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A73" s="1">
         <v>1073</v>
       </c>
@@ -5459,7 +5462,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="74" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A74" s="1">
         <v>1074</v>
       </c>
@@ -5506,7 +5509,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="75" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A75" s="1">
         <v>1075</v>
       </c>
@@ -5553,7 +5556,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="76" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A76" s="1">
         <v>1076</v>
       </c>
@@ -5600,7 +5603,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="77" spans="1:15" ht="34.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:15" ht="25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A77" s="1">
         <v>1077</v>
       </c>
@@ -5647,7 +5650,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="78" spans="1:15" ht="23.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A78" s="1">
         <v>1078</v>
       </c>
@@ -5694,7 +5697,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="79" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A79" s="1">
         <v>1079</v>
       </c>
@@ -5741,7 +5744,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="80" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A80" s="1">
         <v>1080</v>
       </c>
@@ -5788,7 +5791,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="81" spans="1:15" ht="23.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:15" ht="25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A81" s="1">
         <v>1081</v>
       </c>
@@ -5835,7 +5838,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="82" spans="1:15" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:15" ht="49" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A82" s="1">
         <v>1082</v>
       </c>
@@ -5882,7 +5885,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="83" spans="1:15" ht="23.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:15" ht="25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A83" s="1">
         <v>1083</v>
       </c>
@@ -5929,7 +5932,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="84" spans="1:15" ht="23.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:15" ht="25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A84" s="1">
         <v>1084</v>
       </c>
@@ -5976,7 +5979,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="85" spans="1:15" ht="23.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:15" ht="25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A85" s="1">
         <v>1085</v>
       </c>
@@ -6023,7 +6026,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="86" spans="1:15" ht="23.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:15" ht="25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A86" s="1">
         <v>1086</v>
       </c>
@@ -6070,7 +6073,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="87" spans="1:15" ht="23.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A87" s="1">
         <v>1087</v>
       </c>
@@ -6117,7 +6120,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="88" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A88" s="1">
         <v>1088</v>
       </c>
@@ -6164,7 +6167,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="89" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A89" s="1">
         <v>1089</v>
       </c>
@@ -6211,7 +6214,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="90" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A90" s="1">
         <v>1090</v>
       </c>
@@ -6258,7 +6261,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="91" spans="1:15" ht="23.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:15" ht="25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A91" s="1">
         <v>1091</v>
       </c>
@@ -6305,7 +6308,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="92" spans="1:15" ht="57" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:15" ht="61" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A92" s="1">
         <v>1092</v>
       </c>
@@ -6352,7 +6355,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="93" spans="1:15" ht="23.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:15" ht="25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A93" s="1">
         <v>1093</v>
       </c>
@@ -6399,7 +6402,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="94" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A94" s="1">
         <v>1094</v>
       </c>
@@ -6446,7 +6449,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="95" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A95" s="1">
         <v>1095</v>
       </c>
@@ -6493,7 +6496,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="96" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A96" s="1">
         <v>1096</v>
       </c>
@@ -6540,7 +6543,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="97" spans="1:15" ht="23.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A97" s="1">
         <v>1097</v>
       </c>
@@ -6587,7 +6590,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="98" spans="1:15" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:15" ht="49" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A98" s="1">
         <v>1098</v>
       </c>
@@ -6634,7 +6637,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="99" spans="1:15" ht="34.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:15" ht="37" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A99" s="1">
         <v>1099</v>
       </c>
@@ -6681,7 +6684,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="100" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A100" s="1">
         <v>1100</v>
       </c>
@@ -6728,7 +6731,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="101" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A101" s="1">
         <v>1101</v>
       </c>
@@ -6775,7 +6778,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="102" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A102" s="1">
         <v>1102</v>
       </c>
@@ -6822,7 +6825,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="103" spans="1:15" ht="34.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:15" ht="25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A103" s="1">
         <v>1103</v>
       </c>
@@ -6869,7 +6872,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="104" spans="1:15" ht="23.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A104" s="1">
         <v>1104</v>
       </c>
@@ -6916,7 +6919,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="105" spans="1:15" ht="23.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A105" s="1">
         <v>1105</v>
       </c>
@@ -6963,7 +6966,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="106" spans="1:15" ht="34.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:15" ht="25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A106" s="1">
         <v>1106</v>
       </c>
@@ -7010,7 +7013,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="107" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A107" s="1">
         <v>1107</v>
       </c>
@@ -7057,7 +7060,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="108" spans="1:15" ht="23.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:15" ht="25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A108" s="1">
         <v>1108</v>
       </c>
@@ -7104,7 +7107,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="109" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A109" s="1">
         <v>1109</v>
       </c>
@@ -7151,7 +7154,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="110" spans="1:15" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:15" ht="37" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A110" s="1">
         <v>1110</v>
       </c>
@@ -7198,7 +7201,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="111" spans="1:15" ht="23.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:15" ht="25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A111" s="1">
         <v>1111</v>
       </c>
@@ -7245,7 +7248,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="112" spans="1:15" ht="57" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:15" ht="49" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A112" s="1">
         <v>1112</v>
       </c>
@@ -7292,7 +7295,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="113" spans="1:15" ht="57" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:15" ht="49" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A113" s="1">
         <v>1113</v>
       </c>
@@ -7339,7 +7342,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="114" spans="1:15" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:15" ht="37" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A114" s="1">
         <v>1114</v>
       </c>
@@ -7386,7 +7389,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="115" spans="1:15" ht="23.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:15" ht="25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A115" s="1">
         <v>1115</v>
       </c>
@@ -7433,7 +7436,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="116" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A116" s="1">
         <v>1116</v>
       </c>
@@ -7480,7 +7483,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="117" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A117" s="1">
         <v>1117</v>
       </c>
@@ -7527,7 +7530,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="118" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A118" s="1">
         <v>1118</v>
       </c>
@@ -7574,7 +7577,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="119" spans="1:15" ht="23.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:15" ht="25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A119" s="1">
         <v>1119</v>
       </c>
@@ -7621,7 +7624,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="120" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A120" s="1">
         <v>1120</v>
       </c>
@@ -7668,7 +7671,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="121" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A121" s="1">
         <v>1121</v>
       </c>
@@ -7715,7 +7718,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="122" spans="1:15" ht="23.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A122" s="1">
         <v>1122</v>
       </c>
@@ -7762,7 +7765,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="123" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A123" s="1">
         <v>1123</v>
       </c>
@@ -7809,7 +7812,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="124" spans="1:15" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:15" ht="37" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A124" s="1">
         <v>1124</v>
       </c>
@@ -7856,7 +7859,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="125" spans="1:15" ht="23.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:15" ht="25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A125" s="1">
         <v>1125</v>
       </c>
@@ -7903,7 +7906,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="126" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A126" s="1">
         <v>1126</v>
       </c>
@@ -7950,7 +7953,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="127" spans="1:15" ht="23.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:15" ht="25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A127" s="1">
         <v>1127</v>
       </c>
@@ -7997,7 +8000,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="128" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A128" s="1">
         <v>1128</v>
       </c>
@@ -8044,7 +8047,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="129" spans="1:15" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:15" ht="37" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A129" s="1">
         <v>1129</v>
       </c>
@@ -8091,7 +8094,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="130" spans="1:15" ht="34.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:15" ht="25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A130" s="1">
         <v>1130</v>
       </c>
@@ -8138,7 +8141,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="131" spans="1:15" ht="23.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:15" ht="25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A131" s="1">
         <v>1131</v>
       </c>
@@ -8185,7 +8188,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="132" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A132" s="1">
         <v>1132</v>
       </c>
@@ -8232,7 +8235,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="133" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A133" s="1">
         <v>1133</v>
       </c>
@@ -8279,7 +8282,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="134" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A134" s="1">
         <v>1134</v>
       </c>
@@ -8326,7 +8329,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="135" spans="1:15" ht="23.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A135" s="1">
         <v>1135</v>
       </c>
@@ -8373,7 +8376,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="136" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A136" s="1">
         <v>1136</v>
       </c>
@@ -8420,7 +8423,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="137" spans="1:15" ht="23.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:15" ht="25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A137" s="1">
         <v>1137</v>
       </c>
@@ -8467,7 +8470,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="138" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A138" s="1">
         <v>1138</v>
       </c>
@@ -8514,7 +8517,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="139" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A139" s="1">
         <v>1139</v>
       </c>
@@ -8561,7 +8564,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="140" spans="1:15" ht="23.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A140" s="1">
         <v>1140</v>
       </c>
@@ -8608,7 +8611,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="141" spans="1:15" ht="23.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:15" ht="25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A141" s="1">
         <v>1141</v>
       </c>
@@ -8655,7 +8658,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="142" spans="1:15" ht="57" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:15" ht="61" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A142" s="1">
         <v>1142</v>
       </c>
@@ -8702,7 +8705,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="143" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A143" s="1">
         <v>1143</v>
       </c>
@@ -8749,7 +8752,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="144" spans="1:15" ht="34.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:15" ht="25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A144" s="1">
         <v>1144</v>
       </c>
@@ -8796,7 +8799,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="145" spans="1:15" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:15" ht="49" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A145" s="1">
         <v>1145</v>
       </c>
@@ -8843,7 +8846,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="146" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A146" s="1">
         <v>1146</v>
       </c>
@@ -8890,7 +8893,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="147" spans="1:15" ht="23.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:15" ht="25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A147" s="1">
         <v>1147</v>
       </c>
@@ -8937,7 +8940,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="148" spans="1:15" ht="34.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:15" ht="25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A148" s="1">
         <v>1148</v>
       </c>
@@ -8984,7 +8987,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="149" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A149" s="1">
         <v>1149</v>
       </c>
@@ -9031,7 +9034,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="150" spans="1:15" ht="57" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:15" ht="49" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A150" s="1">
         <v>1150</v>
       </c>
@@ -9078,7 +9081,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="151" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A151" s="1">
         <v>1151</v>
       </c>
@@ -9125,7 +9128,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="152" spans="1:15" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:15" ht="37" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A152" s="1">
         <v>1152</v>
       </c>
@@ -9172,7 +9175,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="153" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A153" s="1">
         <v>1153</v>
       </c>
@@ -9219,7 +9222,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="154" spans="1:15" ht="34.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:15" ht="25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A154" s="1">
         <v>1154</v>
       </c>
@@ -9266,7 +9269,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="155" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A155" s="1">
         <v>1155</v>
       </c>
@@ -9313,7 +9316,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="156" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A156" s="1">
         <v>1156</v>
       </c>
@@ -9360,7 +9363,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="157" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A157" s="1">
         <v>1157</v>
       </c>
@@ -9407,7 +9410,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="158" spans="1:15" ht="23.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:15" ht="25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A158" s="1">
         <v>1158</v>
       </c>
@@ -9454,7 +9457,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="159" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A159" s="1">
         <v>1159</v>
       </c>
@@ -9501,7 +9504,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="160" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A160" s="1">
         <v>1160</v>
       </c>
@@ -9548,7 +9551,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="161" spans="1:15" ht="23.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:15" ht="25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A161" s="1">
         <v>1161</v>
       </c>
@@ -9595,7 +9598,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="162" spans="1:15" ht="34.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:15" ht="25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A162" s="1">
         <v>1162</v>
       </c>
@@ -9642,7 +9645,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="163" spans="1:15" ht="23.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A163" s="1">
         <v>1163</v>
       </c>
@@ -9689,7 +9692,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="164" spans="1:15" ht="34.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:15" ht="25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A164" s="1">
         <v>1164</v>
       </c>
@@ -9736,7 +9739,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="165" spans="1:15" ht="34.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:15" ht="25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A165" s="1">
         <v>1165</v>
       </c>
@@ -9783,7 +9786,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="166" spans="1:15" ht="57" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:15" ht="49" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A166" s="1">
         <v>1166</v>
       </c>
@@ -9830,7 +9833,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="167" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A167" s="1">
         <v>1167</v>
       </c>
@@ -9877,7 +9880,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="168" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A168" s="1">
         <v>1168</v>
       </c>
@@ -9924,7 +9927,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="169" spans="1:15" ht="23.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A169" s="1">
         <v>1169</v>
       </c>
@@ -9971,7 +9974,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="170" spans="1:15" ht="23.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:15" ht="25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A170" s="1">
         <v>1170</v>
       </c>
@@ -10018,7 +10021,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="171" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A171" s="1">
         <v>1171</v>
       </c>
@@ -10065,7 +10068,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="172" spans="1:15" ht="23.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:15" ht="25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A172" s="1">
         <v>1172</v>
       </c>
@@ -10112,7 +10115,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="173" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A173" s="1">
         <v>1173</v>
       </c>
@@ -10159,7 +10162,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="174" spans="1:15" ht="57" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:15" ht="49" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A174" s="1">
         <v>1174</v>
       </c>
@@ -10206,7 +10209,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="175" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A175" s="1">
         <v>1175</v>
       </c>
@@ -10253,7 +10256,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="176" spans="1:15" ht="68.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:15" ht="49" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A176" s="1">
         <v>1176</v>
       </c>
@@ -10300,7 +10303,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="177" spans="1:15" ht="23.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:15" ht="25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A177" s="1">
         <v>1177</v>
       </c>
@@ -10347,7 +10350,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="178" spans="1:15" ht="23.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A178" s="1">
         <v>1178</v>
       </c>
@@ -10394,7 +10397,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="179" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A179" s="1">
         <v>1179</v>
       </c>
@@ -10441,7 +10444,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="180" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A180" s="1">
         <v>1180</v>
       </c>
@@ -10488,7 +10491,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="181" spans="1:15" ht="34.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:15" ht="37" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A181" s="1">
         <v>1181</v>
       </c>
@@ -10535,7 +10538,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="182" spans="1:15" ht="57" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:15" ht="49" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A182" s="1">
         <v>1182</v>
       </c>
@@ -10582,7 +10585,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="183" spans="1:15" ht="23.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:15" ht="25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A183" s="1">
         <v>1183</v>
       </c>
@@ -10629,7 +10632,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="184" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A184" s="1">
         <v>1184</v>
       </c>
@@ -10676,7 +10679,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="185" spans="1:15" ht="23.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:15" ht="25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A185" s="1">
         <v>1185</v>
       </c>
@@ -10723,7 +10726,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="186" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A186" s="1">
         <v>1186</v>
       </c>
@@ -10770,7 +10773,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="187" spans="1:15" ht="23.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:15" ht="25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A187" s="1">
         <v>1187</v>
       </c>
@@ -10817,7 +10820,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="188" spans="1:15" ht="23.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A188" s="1">
         <v>1188</v>
       </c>
@@ -10864,7 +10867,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="189" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A189" s="1">
         <v>1189</v>
       </c>
@@ -10911,7 +10914,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="190" spans="1:15" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="190" spans="1:15" ht="37" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A190" s="1">
         <v>1190</v>
       </c>
@@ -10958,7 +10961,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="191" spans="1:15" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="191" spans="1:15" ht="37" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A191" s="1">
         <v>1191</v>
       </c>
@@ -11005,7 +11008,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="192" spans="1:15" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="192" spans="1:15" ht="49" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A192" s="1">
         <v>1192</v>
       </c>
@@ -11052,7 +11055,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="193" spans="1:15" ht="34.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:15" ht="25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A193" s="1">
         <v>1193</v>
       </c>
@@ -11099,7 +11102,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="194" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="194" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A194" s="1">
         <v>1194</v>
       </c>
@@ -11146,7 +11149,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="195" spans="1:15" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="195" spans="1:15" ht="37" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A195" s="1">
         <v>1195</v>
       </c>
@@ -11193,7 +11196,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="196" spans="1:15" ht="23.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="196" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A196" s="1">
         <v>1196</v>
       </c>
@@ -11240,7 +11243,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="197" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="197" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A197" s="1">
         <v>1197</v>
       </c>
@@ -11287,7 +11290,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="198" spans="1:15" ht="23.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="198" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A198" s="1">
         <v>1198</v>
       </c>
@@ -11334,7 +11337,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="199" spans="1:15" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="199" spans="1:15" ht="85" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A199" s="1">
         <v>1199</v>
       </c>
@@ -11381,7 +11384,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="200" spans="1:15" ht="23.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="200" spans="1:15" ht="25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A200" s="1">
         <v>1200</v>
       </c>
@@ -11428,7 +11431,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="201" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="201" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A201" s="1">
         <v>1201</v>
       </c>
@@ -11475,7 +11478,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="202" spans="1:15" ht="113.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="202" spans="1:15" ht="121" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A202" s="1">
         <v>1202</v>
       </c>
@@ -11522,7 +11525,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="203" spans="1:15" ht="23.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="203" spans="1:15" ht="25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A203" s="1">
         <v>1203</v>
       </c>
@@ -11569,7 +11572,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="204" spans="1:15" ht="34.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="204" spans="1:15" ht="25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A204" s="1">
         <v>1204</v>
       </c>
@@ -11616,7 +11619,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="205" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="205" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A205" s="1">
         <v>1205</v>
       </c>
@@ -11663,7 +11666,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="206" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="206" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A206" s="1">
         <v>1206</v>
       </c>
@@ -11710,7 +11713,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="207" spans="1:15" ht="23.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="207" spans="1:15" ht="25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A207" s="1">
         <v>1207</v>
       </c>
@@ -11757,7 +11760,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="208" spans="1:15" ht="23.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="208" spans="1:15" ht="25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A208" s="1">
         <v>1208</v>
       </c>
@@ -11804,7 +11807,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="209" spans="1:15" ht="34.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="209" spans="1:15" ht="37" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A209" s="1">
         <v>1209</v>
       </c>
@@ -11851,7 +11854,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="210" spans="1:15" ht="34.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="210" spans="1:15" ht="37" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A210" s="1">
         <v>1210</v>
       </c>
@@ -11898,7 +11901,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="211" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="211" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A211" s="1">
         <v>1211</v>
       </c>
@@ -11945,7 +11948,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="212" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="212" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A212" s="1">
         <v>1212</v>
       </c>
@@ -11992,7 +11995,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="213" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="213" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A213" s="1">
         <v>1213</v>
       </c>
@@ -12039,7 +12042,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="214" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="214" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A214" s="1">
         <v>1214</v>
       </c>
@@ -12086,7 +12089,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="215" spans="1:15" ht="23.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="215" spans="1:15" ht="25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A215" s="1">
         <v>1215</v>
       </c>
@@ -12133,7 +12136,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="216" spans="1:15" ht="113.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="216" spans="1:15" ht="97" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A216" s="1">
         <v>1216</v>
       </c>
@@ -12180,7 +12183,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="217" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="217" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A217" s="1">
         <v>1217</v>
       </c>
@@ -12227,7 +12230,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="218" spans="1:15" ht="23.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="218" spans="1:15" ht="25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A218" s="1">
         <v>1218</v>
       </c>
@@ -12274,7 +12277,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="219" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="219" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A219" s="1">
         <v>1219</v>
       </c>
@@ -12321,7 +12324,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="220" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="220" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A220" s="1">
         <v>1220</v>
       </c>
@@ -12368,7 +12371,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="221" spans="1:15" ht="23.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="221" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A221" s="1">
         <v>1221</v>
       </c>
@@ -12415,7 +12418,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="222" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="222" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A222" s="1">
         <v>1222</v>
       </c>
@@ -12462,7 +12465,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="223" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="223" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A223" s="1">
         <v>1223</v>
       </c>
@@ -12509,7 +12512,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="224" spans="1:15" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="224" spans="1:15" ht="37" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A224" s="1">
         <v>1224</v>
       </c>
@@ -12556,7 +12559,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="225" spans="1:15" ht="23.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="225" spans="1:15" ht="25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A225" s="1">
         <v>1225</v>
       </c>
@@ -12603,7 +12606,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="226" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="226" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A226" s="1">
         <v>1226</v>
       </c>
@@ -12650,7 +12653,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="227" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="227" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A227" s="1">
         <v>1227</v>
       </c>
@@ -12697,7 +12700,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="228" spans="1:15" ht="23.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="228" spans="1:15" ht="25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A228" s="1">
         <v>1228</v>
       </c>
@@ -12744,7 +12747,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="229" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="229" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A229" s="1">
         <v>1229</v>
       </c>
@@ -12791,7 +12794,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="230" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="230" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A230" s="1">
         <v>1230</v>
       </c>
@@ -12838,7 +12841,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="231" spans="1:15" ht="23.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="231" spans="1:15" ht="25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A231" s="1">
         <v>1231</v>
       </c>
@@ -12885,7 +12888,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="232" spans="1:15" ht="23.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="232" spans="1:15" ht="25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A232" s="1">
         <v>1232</v>
       </c>
@@ -12932,7 +12935,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="233" spans="1:15" ht="34.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="233" spans="1:15" ht="37" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A233" s="1">
         <v>1233</v>
       </c>
@@ -12979,7 +12982,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="234" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="234" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A234" s="1">
         <v>1234</v>
       </c>
@@ -13026,7 +13029,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="235" spans="1:15" ht="23.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="235" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A235" s="1">
         <v>1235</v>
       </c>
@@ -13073,7 +13076,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="236" spans="1:15" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="236" spans="1:15" ht="37" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A236" s="1">
         <v>1236</v>
       </c>
@@ -13120,7 +13123,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="237" spans="1:15" ht="23.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="237" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A237" s="1">
         <v>1237</v>
       </c>
@@ -13167,7 +13170,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="238" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="238" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A238" s="1">
         <v>1238</v>
       </c>
@@ -13214,7 +13217,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="239" spans="1:15" ht="23.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="239" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A239" s="1">
         <v>1239</v>
       </c>
@@ -13261,7 +13264,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="240" spans="1:15" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="240" spans="1:15" ht="37" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A240" s="1">
         <v>1240</v>
       </c>
@@ -13308,7 +13311,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="241" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="241" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A241" s="1">
         <v>1241</v>
       </c>
@@ -13355,7 +13358,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="242" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="242" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A242" s="1">
         <v>1242</v>
       </c>
@@ -13402,7 +13405,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="243" spans="1:15" ht="23.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="243" spans="1:15" ht="25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A243" s="1">
         <v>1243</v>
       </c>
@@ -13449,7 +13452,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="244" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="244" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A244" s="1">
         <v>1244</v>
       </c>
@@ -13496,7 +13499,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="245" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="245" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A245" s="1">
         <v>1245</v>
       </c>
@@ -13543,7 +13546,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="246" spans="1:15" ht="34.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="246" spans="1:15" ht="37" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A246" s="1">
         <v>1246</v>
       </c>
@@ -13590,7 +13593,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="247" spans="1:15" ht="57" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="247" spans="1:15" ht="61" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A247" s="1">
         <v>1247</v>
       </c>
@@ -13637,7 +13640,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="248" spans="1:15" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="248" spans="1:15" ht="37" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A248" s="1">
         <v>1248</v>
       </c>
@@ -13684,7 +13687,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="249" spans="1:15" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="249" spans="1:15" ht="37" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A249" s="1">
         <v>1249</v>
       </c>
@@ -13731,7 +13734,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="250" spans="1:15" ht="23.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="250" spans="1:15" ht="25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A250" s="1">
         <v>1250</v>
       </c>
@@ -13778,7 +13781,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="251" spans="1:15" ht="23.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="251" spans="1:15" ht="25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A251" s="1">
         <v>1251</v>
       </c>
@@ -13825,7 +13828,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="252" spans="1:15" ht="79.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="252" spans="1:15" ht="85" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A252" s="1">
         <v>1252</v>
       </c>
@@ -13872,7 +13875,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="253" spans="1:15" ht="68.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="253" spans="1:15" ht="61" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A253" s="1">
         <v>1253</v>
       </c>
@@ -13919,7 +13922,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="254" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="254" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A254" s="1">
         <v>1254</v>
       </c>
@@ -13966,7 +13969,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="255" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="255" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A255" s="1">
         <v>1255</v>
       </c>
@@ -14013,7 +14016,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="256" spans="1:15" ht="23.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="256" spans="1:15" ht="25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A256" s="1">
         <v>1256</v>
       </c>
@@ -14060,7 +14063,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="257" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="257" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A257" s="1">
         <v>1257</v>
       </c>
@@ -14107,7 +14110,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="258" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="258" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A258" s="1">
         <v>1258</v>
       </c>
@@ -14154,7 +14157,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="259" spans="1:15" ht="23.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="259" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A259" s="1">
         <v>1259</v>
       </c>
@@ -14201,7 +14204,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="260" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="260" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A260" s="1">
         <v>1260</v>
       </c>
@@ -14248,7 +14251,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="261" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="261" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A261" s="1">
         <v>1261</v>
       </c>
@@ -14295,7 +14298,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="262" spans="1:15" ht="34.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="262" spans="1:15" ht="25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A262" s="1">
         <v>1262</v>
       </c>
@@ -14342,7 +14345,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="263" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="263" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A263" s="1">
         <v>1263</v>
       </c>
@@ -14389,7 +14392,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="264" spans="1:15" ht="34.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="264" spans="1:15" ht="25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A264" s="1">
         <v>1264</v>
       </c>
@@ -14436,7 +14439,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="265" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="265" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A265" s="1">
         <v>1265</v>
       </c>
@@ -14483,7 +14486,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="266" spans="1:15" ht="79.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="266" spans="1:15" ht="61" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A266" s="1">
         <v>1266</v>
       </c>
@@ -14530,7 +14533,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="267" spans="1:15" ht="23.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="267" spans="1:15" ht="25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A267" s="1">
         <v>1267</v>
       </c>
@@ -14577,7 +14580,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="268" spans="1:15" ht="23.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="268" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A268" s="1">
         <v>1268</v>
       </c>
@@ -14624,7 +14627,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="269" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="269" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A269" s="1">
         <v>1269</v>
       </c>
@@ -14671,7 +14674,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="270" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="270" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A270" s="1">
         <v>1270</v>
       </c>
@@ -14718,7 +14721,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="271" spans="1:15" ht="23.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="271" spans="1:15" ht="25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A271" s="1">
         <v>1271</v>
       </c>
@@ -14765,7 +14768,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="272" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="272" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A272" s="1">
         <v>1272</v>
       </c>
@@ -14812,7 +14815,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="273" spans="1:15" ht="34.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="273" spans="1:15" ht="25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A273" s="1">
         <v>1273</v>
       </c>
@@ -14859,7 +14862,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="274" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="274" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A274" s="1">
         <v>1274</v>
       </c>
@@ -14906,7 +14909,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="275" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="275" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A275" s="1">
         <v>1275</v>
       </c>
@@ -14953,7 +14956,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="276" spans="1:15" ht="34.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="276" spans="1:15" ht="25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A276" s="1">
         <v>1276</v>
       </c>
@@ -15000,7 +15003,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="277" spans="1:15" ht="34.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="277" spans="1:15" ht="25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A277" s="1">
         <v>1277</v>
       </c>
@@ -15047,7 +15050,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="278" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="278" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A278" s="1">
         <v>1278</v>
       </c>
@@ -15094,7 +15097,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="279" spans="1:15" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="279" spans="1:15" ht="37" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A279" s="1">
         <v>1279</v>
       </c>
@@ -15141,7 +15144,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="280" spans="1:15" ht="23.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="280" spans="1:15" ht="25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A280" s="1">
         <v>1280</v>
       </c>
@@ -15188,7 +15191,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="281" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="281" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A281" s="1">
         <v>1281</v>
       </c>
@@ -15235,7 +15238,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="282" spans="1:15" ht="23.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="282" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A282" s="1">
         <v>1282</v>
       </c>
@@ -15282,7 +15285,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="283" spans="1:15" ht="23.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="283" spans="1:15" ht="25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A283" s="1">
         <v>1283</v>
       </c>
@@ -15329,7 +15332,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="284" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="284" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A284" s="1">
         <v>1284</v>
       </c>
@@ -15376,7 +15379,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="285" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="285" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A285" s="1">
         <v>1285</v>
       </c>
@@ -15423,7 +15426,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="286" spans="1:15" ht="79.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="286" spans="1:15" ht="73" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A286" s="1">
         <v>1286</v>
       </c>
@@ -15470,7 +15473,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="287" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="287" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A287" s="1">
         <v>1287</v>
       </c>
@@ -15517,7 +15520,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="288" spans="1:15" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="288" spans="1:15" ht="25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A288" s="1">
         <v>1288</v>
       </c>
@@ -15564,7 +15567,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="289" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="289" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A289" s="1">
         <v>1289</v>
       </c>
@@ -15611,7 +15614,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="290" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="290" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A290" s="1">
         <v>1290</v>
       </c>
@@ -15658,7 +15661,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="291" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="291" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A291" s="1">
         <v>1291</v>
       </c>
@@ -15705,7 +15708,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="292" spans="1:15" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="292" spans="1:15" ht="37" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A292" s="1">
         <v>1292</v>
       </c>
@@ -15752,7 +15755,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="293" spans="1:15" ht="34.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="293" spans="1:15" ht="25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A293" s="1">
         <v>1293</v>
       </c>
@@ -15799,7 +15802,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="294" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="294" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A294" s="1">
         <v>1294</v>
       </c>
@@ -15846,7 +15849,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="295" spans="1:15" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="295" spans="1:15" ht="37" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A295" s="1">
         <v>1295</v>
       </c>
@@ -15893,7 +15896,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="296" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="296" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A296" s="1">
         <v>1296</v>
       </c>
@@ -15940,7 +15943,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="297" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="297" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A297" s="1">
         <v>1297</v>
       </c>
@@ -15987,7 +15990,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="298" spans="1:15" ht="23.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="298" spans="1:15" ht="25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A298" s="1">
         <v>1298</v>
       </c>
@@ -16034,7 +16037,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="299" spans="1:15" ht="23.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="299" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A299" s="1">
         <v>1299</v>
       </c>
@@ -16081,7 +16084,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="300" spans="1:15" ht="23.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="300" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A300" s="1">
         <v>1300</v>
       </c>
@@ -16128,7 +16131,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="301" spans="1:15" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="301" spans="1:15" ht="37" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A301" s="1">
         <v>1301</v>
       </c>
@@ -16175,7 +16178,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="302" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="302" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A302" s="1">
         <v>1302</v>
       </c>
@@ -16222,7 +16225,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="303" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="303" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A303" s="1">
         <v>1303</v>
       </c>
@@ -16269,7 +16272,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="304" spans="1:15" ht="34.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="304" spans="1:15" ht="25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A304" s="1">
         <v>1304</v>
       </c>
@@ -16316,7 +16319,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="305" spans="1:15" ht="23.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="305" spans="1:15" ht="25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A305" s="1">
         <v>1305</v>
       </c>
@@ -16363,7 +16366,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="306" spans="1:15" ht="34.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="306" spans="1:15" ht="25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A306" s="1">
         <v>1306</v>
       </c>
@@ -16410,7 +16413,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="307" spans="1:15" ht="23.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="307" spans="1:15" ht="25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A307" s="1">
         <v>1307</v>
       </c>
@@ -16457,7 +16460,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="308" spans="1:15" ht="57" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="308" spans="1:15" ht="37" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A308" s="1">
         <v>1308</v>
       </c>
@@ -16504,7 +16507,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="309" spans="1:15" ht="34.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="309" spans="1:15" ht="37" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A309" s="1">
         <v>1309</v>
       </c>
@@ -16551,7 +16554,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="310" spans="1:15" ht="23.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="310" spans="1:15" ht="25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A310" s="1">
         <v>1310</v>
       </c>
@@ -16598,7 +16601,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="311" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="311" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A311" s="1">
         <v>1311</v>
       </c>
@@ -16645,7 +16648,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="312" spans="1:15" ht="34.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="312" spans="1:15" ht="25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A312" s="1">
         <v>1312</v>
       </c>
@@ -16692,7 +16695,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="313" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="313" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A313" s="1">
         <v>1313</v>
       </c>
@@ -16720,8 +16723,8 @@
       <c r="I313" s="1">
         <v>-6</v>
       </c>
-      <c r="J313" s="1">
-        <v>9</v>
+      <c r="J313" s="1" t="s">
+        <v>527</v>
       </c>
       <c r="K313" s="1">
         <v>22</v>
@@ -16739,7 +16742,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="314" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="314" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A314" s="1">
         <v>1314</v>
       </c>
@@ -16786,7 +16789,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="315" spans="1:15" ht="23.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="315" spans="1:15" ht="25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A315" s="1">
         <v>1315</v>
       </c>
@@ -16833,7 +16836,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="316" spans="1:15" ht="23.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="316" spans="1:15" ht="25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A316" s="1">
         <v>1316</v>
       </c>
@@ -16880,7 +16883,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="317" spans="1:15" ht="23.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="317" spans="1:15" ht="25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A317" s="1">
         <v>1317</v>
       </c>
@@ -16927,7 +16930,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="318" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="318" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A318" s="1">
         <v>1318</v>
       </c>
@@ -16986,16 +16989,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACA8EEAF-72C1-4AF2-B1F2-7BB9A7433E9F}">
   <dimension ref="A1:B28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B25" sqref="B2:B25"/>
+    <sheetView topLeftCell="A9" zoomScale="213" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="11.5703125" customWidth="1"/>
+    <col min="2" max="2" width="11.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="23.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>518</v>
       </c>
@@ -17003,7 +17006,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>101</v>
       </c>
@@ -17011,7 +17014,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>102</v>
       </c>
@@ -17019,7 +17022,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>103</v>
       </c>
@@ -17027,7 +17030,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>104</v>
       </c>
@@ -17035,7 +17038,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>105</v>
       </c>
@@ -17043,7 +17046,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>106</v>
       </c>
@@ -17051,7 +17054,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>107</v>
       </c>
@@ -17059,7 +17062,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>121</v>
       </c>
@@ -17067,7 +17070,7 @@
         <v>524</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="23.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>108</v>
       </c>
@@ -17075,7 +17078,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>109</v>
       </c>
@@ -17083,7 +17086,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="23.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>115</v>
       </c>
@@ -17091,7 +17094,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="13" spans="1:2" ht="23.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:2" ht="25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>120</v>
       </c>
@@ -17099,7 +17102,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="14" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:2" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>110</v>
       </c>
@@ -17107,7 +17110,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="15" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:2" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>111</v>
       </c>
@@ -17115,7 +17118,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="16" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:2" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>112</v>
       </c>
@@ -17123,7 +17126,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:2" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>113</v>
       </c>
@@ -17131,7 +17134,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="18" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:2" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>114</v>
       </c>
@@ -17139,7 +17142,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="19" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:2" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>115</v>
       </c>
@@ -17147,7 +17150,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="20" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:2" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>116</v>
       </c>
@@ -17155,7 +17158,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="21" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:2" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>123</v>
       </c>
@@ -17163,7 +17166,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="22" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:2" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>117</v>
       </c>
@@ -17171,7 +17174,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="23" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:2" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>118</v>
       </c>
@@ -17179,7 +17182,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="24" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:2" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>124</v>
       </c>
@@ -17187,7 +17190,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="25" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:2" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>119</v>
       </c>
@@ -17195,13 +17198,13 @@
         <v>95</v>
       </c>
     </row>
-    <row r="26" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:2" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B26" s="1"/>
     </row>
-    <row r="27" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:2" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B27" s="1"/>
     </row>
-    <row r="28" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:2" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B28" s="1"/>
     </row>
   </sheetData>
@@ -17216,17 +17219,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA67EFAF-51EF-459E-A758-A3C9E857DDED}">
   <dimension ref="A1:C171"/>
   <sheetViews>
-    <sheetView topLeftCell="A97" workbookViewId="0">
-      <selection activeCell="A109" sqref="A109:XFD109"/>
+    <sheetView zoomScale="99" workbookViewId="0">
+      <selection activeCell="B106" sqref="B106"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="18.42578125" customWidth="1"/>
-    <col min="3" max="3" width="12.5703125" customWidth="1"/>
+    <col min="2" max="2" width="18.5" customWidth="1"/>
+    <col min="3" max="3" width="12.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="23.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>521</v>
       </c>
@@ -17237,7 +17240,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -17248,7 +17251,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -17259,7 +17262,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="23.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -17270,7 +17273,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -17281,7 +17284,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="23.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -17292,7 +17295,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -17303,7 +17306,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -17314,7 +17317,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -17325,7 +17328,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -17336,7 +17339,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -17347,7 +17350,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -17358,7 +17361,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -17369,7 +17372,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="23.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>13</v>
       </c>
@@ -17380,7 +17383,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>14</v>
       </c>
@@ -17391,7 +17394,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>15</v>
       </c>
@@ -17402,7 +17405,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>16</v>
       </c>
@@ -17413,7 +17416,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>17</v>
       </c>
@@ -17424,7 +17427,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>18</v>
       </c>
@@ -17435,7 +17438,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>19</v>
       </c>
@@ -17446,7 +17449,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>20</v>
       </c>
@@ -17457,7 +17460,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>21</v>
       </c>
@@ -17468,7 +17471,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>22</v>
       </c>
@@ -17479,7 +17482,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>23</v>
       </c>
@@ -17490,7 +17493,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>24</v>
       </c>
@@ -17501,7 +17504,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>25</v>
       </c>
@@ -17512,7 +17515,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>26</v>
       </c>
@@ -17523,7 +17526,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>27</v>
       </c>
@@ -17534,7 +17537,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>28</v>
       </c>
@@ -17545,7 +17548,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>29</v>
       </c>
@@ -17556,7 +17559,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>30</v>
       </c>
@@ -17567,7 +17570,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>31</v>
       </c>
@@ -17578,7 +17581,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>32</v>
       </c>
@@ -17589,7 +17592,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="34" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>33</v>
       </c>
@@ -17600,7 +17603,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>34</v>
       </c>
@@ -17611,7 +17614,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>35</v>
       </c>
@@ -17622,7 +17625,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="37" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>36</v>
       </c>
@@ -17633,7 +17636,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="38" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>37</v>
       </c>
@@ -17644,7 +17647,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="39" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>38</v>
       </c>
@@ -17655,7 +17658,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="40" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>39</v>
       </c>
@@ -17666,7 +17669,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="41" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>40</v>
       </c>
@@ -17677,7 +17680,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <v>41</v>
       </c>
@@ -17688,7 +17691,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="43" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <v>42</v>
       </c>
@@ -17699,7 +17702,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="44" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <v>43</v>
       </c>
@@ -17710,7 +17713,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="45" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
         <v>44</v>
       </c>
@@ -17721,7 +17724,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="46" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
         <v>45</v>
       </c>
@@ -17732,7 +17735,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="47" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
         <v>46</v>
       </c>
@@ -17743,7 +17746,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="48" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
         <v>47</v>
       </c>
@@ -17754,7 +17757,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="49" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
         <v>48</v>
       </c>
@@ -17765,7 +17768,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
         <v>49</v>
       </c>
@@ -17776,7 +17779,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="51" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
         <v>50</v>
       </c>
@@ -17787,7 +17790,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="52" spans="1:3" ht="34.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
         <v>51</v>
       </c>
@@ -17798,7 +17801,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="53" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
         <v>52</v>
       </c>
@@ -17809,7 +17812,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="54" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
         <v>53</v>
       </c>
@@ -17820,7 +17823,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="55" spans="1:3" ht="23.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
         <v>54</v>
       </c>
@@ -17831,7 +17834,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="56" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
         <v>55</v>
       </c>
@@ -17842,7 +17845,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="57" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
         <v>56</v>
       </c>
@@ -17853,7 +17856,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="58" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
         <v>57</v>
       </c>
@@ -17864,7 +17867,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="59" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A59" s="1">
         <v>58</v>
       </c>
@@ -17875,7 +17878,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="60" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
         <v>59</v>
       </c>
@@ -17886,7 +17889,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="61" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A61" s="1">
         <v>60</v>
       </c>
@@ -17897,7 +17900,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="62" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A62" s="1">
         <v>61</v>
       </c>
@@ -17908,7 +17911,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="63" spans="1:3" ht="23.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A63" s="1">
         <v>62</v>
       </c>
@@ -17919,7 +17922,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="64" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A64" s="1">
         <v>63</v>
       </c>
@@ -17930,7 +17933,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="65" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A65" s="1">
         <v>64</v>
       </c>
@@ -17941,7 +17944,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="66" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A66" s="1">
         <v>65</v>
       </c>
@@ -17952,7 +17955,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="67" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A67" s="1">
         <v>66</v>
       </c>
@@ -17963,7 +17966,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="68" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A68" s="1">
         <v>67</v>
       </c>
@@ -17974,7 +17977,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="69" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A69" s="1">
         <v>68</v>
       </c>
@@ -17985,7 +17988,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="70" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A70" s="1">
         <v>69</v>
       </c>
@@ -17996,7 +17999,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="71" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A71" s="1">
         <v>70</v>
       </c>
@@ -18007,7 +18010,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="72" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A72" s="1">
         <v>71</v>
       </c>
@@ -18018,7 +18021,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="73" spans="1:3" ht="23.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A73" s="1">
         <v>72</v>
       </c>
@@ -18029,7 +18032,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="74" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A74" s="1">
         <v>73</v>
       </c>
@@ -18040,7 +18043,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="75" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A75" s="1">
         <v>74</v>
       </c>
@@ -18051,7 +18054,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="76" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A76" s="1">
         <v>75</v>
       </c>
@@ -18062,7 +18065,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="77" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A77" s="1">
         <v>76</v>
       </c>
@@ -18073,7 +18076,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="78" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A78" s="1">
         <v>77</v>
       </c>
@@ -18084,7 +18087,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="79" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A79" s="1">
         <v>78</v>
       </c>
@@ -18095,7 +18098,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="80" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A80" s="1">
         <v>79</v>
       </c>
@@ -18106,7 +18109,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="81" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A81" s="1">
         <v>80</v>
       </c>
@@ -18117,7 +18120,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="82" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A82" s="1">
         <v>81</v>
       </c>
@@ -18128,7 +18131,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="83" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A83" s="1">
         <v>82</v>
       </c>
@@ -18139,7 +18142,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="84" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A84" s="1">
         <v>83</v>
       </c>
@@ -18150,7 +18153,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="85" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A85" s="1">
         <v>84</v>
       </c>
@@ -18161,7 +18164,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="86" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A86" s="1">
         <v>85</v>
       </c>
@@ -18172,7 +18175,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="87" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A87" s="1">
         <v>86</v>
       </c>
@@ -18183,7 +18186,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="88" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A88" s="1">
         <v>87</v>
       </c>
@@ -18194,7 +18197,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="89" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A89" s="1">
         <v>88</v>
       </c>
@@ -18205,7 +18208,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="90" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A90" s="1">
         <v>89</v>
       </c>
@@ -18216,7 +18219,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="91" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A91" s="1">
         <v>90</v>
       </c>
@@ -18227,7 +18230,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="92" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A92" s="1">
         <v>91</v>
       </c>
@@ -18238,7 +18241,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="93" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A93" s="1">
         <v>92</v>
       </c>
@@ -18249,7 +18252,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="94" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A94" s="1">
         <v>93</v>
       </c>
@@ -18260,7 +18263,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="95" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A95" s="1">
         <v>94</v>
       </c>
@@ -18271,7 +18274,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="96" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A96" s="1">
         <v>95</v>
       </c>
@@ -18282,7 +18285,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="97" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A97" s="1">
         <v>96</v>
       </c>
@@ -18293,7 +18296,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="98" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A98" s="1">
         <v>97</v>
       </c>
@@ -18304,7 +18307,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="99" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A99" s="1">
         <v>98</v>
       </c>
@@ -18315,7 +18318,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="100" spans="1:3" ht="23.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A100" s="1">
         <v>99</v>
       </c>
@@ -18326,7 +18329,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="101" spans="1:3" ht="23.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A101" s="1">
         <v>100</v>
       </c>
@@ -18337,7 +18340,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="102" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A102" s="1">
         <v>101</v>
       </c>
@@ -18348,7 +18351,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="103" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A103" s="1">
         <v>102</v>
       </c>
@@ -18359,7 +18362,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="104" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A104" s="1">
         <v>103</v>
       </c>
@@ -18370,7 +18373,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="105" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A105" s="1">
         <v>104</v>
       </c>
@@ -18381,7 +18384,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="106" spans="1:3" ht="34.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A106" s="1">
         <v>105</v>
       </c>
@@ -18392,7 +18395,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="107" spans="1:3" ht="23.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A107" s="1">
         <v>106</v>
       </c>
@@ -18403,7 +18406,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="108" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A108" s="1">
         <v>107</v>
       </c>
@@ -18414,7 +18417,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="109" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A109" s="1">
         <v>108</v>
       </c>
@@ -18425,7 +18428,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="110" spans="1:3" ht="23.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A110" s="1">
         <v>109</v>
       </c>
@@ -18436,7 +18439,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="111" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A111" s="1">
         <v>110</v>
       </c>
@@ -18447,7 +18450,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="112" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A112" s="1">
         <v>111</v>
       </c>
@@ -18458,7 +18461,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="113" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A113" s="1">
         <v>112</v>
       </c>
@@ -18469,7 +18472,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="114" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A114" s="1">
         <v>113</v>
       </c>
@@ -18480,7 +18483,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="115" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A115" s="1">
         <v>114</v>
       </c>
@@ -18491,7 +18494,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="116" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A116" s="1">
         <v>115</v>
       </c>
@@ -18502,7 +18505,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="117" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A117" s="1">
         <v>116</v>
       </c>
@@ -18513,7 +18516,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="118" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A118" s="1">
         <v>117</v>
       </c>
@@ -18524,7 +18527,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="119" spans="1:3" ht="23.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A119" s="1">
         <v>118</v>
       </c>
@@ -18535,7 +18538,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="120" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A120" s="1">
         <v>119</v>
       </c>
@@ -18546,7 +18549,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="121" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A121" s="1">
         <v>120</v>
       </c>
@@ -18557,7 +18560,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="122" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A122" s="1">
         <v>121</v>
       </c>
@@ -18568,7 +18571,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="123" spans="1:3" ht="23.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A123" s="1">
         <v>122</v>
       </c>
@@ -18579,7 +18582,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="124" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A124" s="1">
         <v>123</v>
       </c>
@@ -18590,7 +18593,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="125" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A125" s="1">
         <v>124</v>
       </c>
@@ -18601,7 +18604,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="126" spans="1:3" ht="23.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A126" s="1">
         <v>125</v>
       </c>
@@ -18612,7 +18615,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="127" spans="1:3" ht="23.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A127" s="1">
         <v>126</v>
       </c>
@@ -18623,7 +18626,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="128" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A128" s="1">
         <v>127</v>
       </c>
@@ -18634,7 +18637,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="129" spans="1:3" ht="23.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A129" s="1">
         <v>128</v>
       </c>
@@ -18645,7 +18648,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="130" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A130" s="1">
         <v>129</v>
       </c>
@@ -18656,7 +18659,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="131" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A131" s="1">
         <v>130</v>
       </c>
@@ -18667,7 +18670,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="132" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A132" s="1">
         <v>131</v>
       </c>
@@ -18678,7 +18681,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="133" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A133" s="1">
         <v>132</v>
       </c>
@@ -18689,7 +18692,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="134" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A134" s="1">
         <v>133</v>
       </c>
@@ -18700,7 +18703,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="135" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A135" s="1">
         <v>134</v>
       </c>
@@ -18711,7 +18714,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="136" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A136" s="1">
         <v>135</v>
       </c>
@@ -18722,7 +18725,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="137" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A137" s="1">
         <v>136</v>
       </c>
@@ -18733,7 +18736,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="138" spans="1:3" ht="23.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A138" s="1">
         <v>137</v>
       </c>
@@ -18744,7 +18747,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="139" spans="1:3" ht="23.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A139" s="1">
         <v>138</v>
       </c>
@@ -18755,7 +18758,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="140" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A140" s="1">
         <v>139</v>
       </c>
@@ -18766,7 +18769,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="141" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A141" s="1">
         <v>140</v>
       </c>
@@ -18777,7 +18780,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="142" spans="1:3" ht="23.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A142" s="1">
         <v>141</v>
       </c>
@@ -18788,7 +18791,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="143" spans="1:3" ht="23.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A143" s="1">
         <v>142</v>
       </c>
@@ -18799,7 +18802,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="144" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A144" s="1">
         <v>143</v>
       </c>
@@ -18810,7 +18813,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="145" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A145" s="1">
         <v>144</v>
       </c>
@@ -18821,7 +18824,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="146" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A146" s="1">
         <v>145</v>
       </c>
@@ -18832,7 +18835,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="147" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A147" s="1">
         <v>146</v>
       </c>
@@ -18843,7 +18846,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="148" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A148" s="1">
         <v>147</v>
       </c>
@@ -18854,7 +18857,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="149" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A149" s="1">
         <v>148</v>
       </c>
@@ -18865,7 +18868,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="150" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A150" s="1">
         <v>149</v>
       </c>
@@ -18876,7 +18879,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="151" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A151" s="1">
         <v>150</v>
       </c>
@@ -18887,7 +18890,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="152" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A152" s="1">
         <v>151</v>
       </c>
@@ -18898,7 +18901,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="153" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A153" s="1">
         <v>152</v>
       </c>
@@ -18909,7 +18912,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="154" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A154" s="1">
         <v>153</v>
       </c>
@@ -18920,7 +18923,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="155" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A155" s="1">
         <v>154</v>
       </c>
@@ -18931,7 +18934,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="156" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A156" s="1">
         <v>155</v>
       </c>
@@ -18942,7 +18945,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="157" spans="1:3" ht="23.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A157" s="1">
         <v>156</v>
       </c>
@@ -18953,7 +18956,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="158" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A158" s="1">
         <v>157</v>
       </c>
@@ -18964,7 +18967,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="159" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A159" s="1">
         <v>158</v>
       </c>
@@ -18975,7 +18978,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="160" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A160" s="1">
         <v>159</v>
       </c>
@@ -18986,7 +18989,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="161" spans="1:3" ht="23.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A161" s="1">
         <v>160</v>
       </c>
@@ -18997,7 +19000,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="162" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A162" s="1">
         <v>161</v>
       </c>
@@ -19008,7 +19011,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="163" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A163" s="1">
         <v>162</v>
       </c>
@@ -19019,7 +19022,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="164" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A164" s="1">
         <v>163</v>
       </c>
@@ -19030,7 +19033,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="165" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A165" s="1">
         <v>164</v>
       </c>
@@ -19041,7 +19044,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="166" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A166" s="1">
         <v>165</v>
       </c>
@@ -19052,7 +19055,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="167" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A167" s="1">
         <v>166</v>
       </c>
@@ -19063,7 +19066,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="168" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A168" s="1">
         <v>167</v>
       </c>
@@ -19074,7 +19077,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="169" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A169" s="1">
         <v>168</v>
       </c>
@@ -19085,7 +19088,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="170" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A170" s="1">
         <v>169</v>
       </c>
@@ -19096,7 +19099,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="171" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A171" s="1">
         <v>170</v>
       </c>
@@ -19120,12 +19123,12 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="12.42578125" customWidth="1"/>
+    <col min="2" max="2" width="12.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="23.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>522</v>
       </c>
@@ -19133,7 +19136,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="22.5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -19141,7 +19144,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -19149,7 +19152,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -19157,7 +19160,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>

</xml_diff>